<commit_message>
Adapt bulac to fleet changes to Uruguay 2025 model
</commit_message>
<xml_diff>
--- a/Taxes_Factors.xlsx
+++ b/Taxes_Factors.xlsx
@@ -463,13 +463,13 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.148151490478081</v>
+        <v>0.1273426742845834</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>0.1774628869167034</v>
+        <v>0.1375864719616154</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0.1661637819774276</v>
+        <v>0.009218662286240091</v>
       </c>
     </row>
     <row r="3">
@@ -479,13 +479,13 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.1715471575587239</v>
+        <v>0.1385664810060629</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.07176647001255382</v>
+        <v>0.07361601420459957</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0.010118724709961</v>
+        <v>0.1608122037454987</v>
       </c>
     </row>
     <row r="4">
@@ -495,13 +495,13 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>0.08429566860895799</v>
+        <v>0.02866171107854141</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.04292839852331825</v>
+        <v>0.1286148203061389</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0.09908086558817701</v>
+        <v>0.1410991310337403</v>
       </c>
     </row>
     <row r="5">
@@ -511,13 +511,13 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>0.0723960141809772</v>
+        <v>0.005599852723031887</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.05278968427940997</v>
+        <v>0.0439363938074464</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>0.04221190078861956</v>
+        <v>0.1681830836057347</v>
       </c>
     </row>
     <row r="6">
@@ -527,13 +527,13 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.1233266328484123</v>
+        <v>0.08988188957996833</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0.01962493450899457</v>
+        <v>0.1059079198305923</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0.05682639186604213</v>
+        <v>0.02792260181143307</v>
       </c>
     </row>
     <row r="7">
@@ -543,13 +543,13 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.0265184256788662</v>
+        <v>0.1108322445897598</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.1556529596948173</v>
+        <v>0.1721514704028065</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0.01699696908463966</v>
+        <v>0.04982390814496991</v>
       </c>
     </row>
     <row r="8">
@@ -559,13 +559,13 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.01073521250169291</v>
+        <v>0.07138001983692742</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0.1078335522942664</v>
+        <v>0.0007266658150443441</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>0.128921668961639</v>
+        <v>0.08715786115037481</v>
       </c>
     </row>
     <row r="9">
@@ -575,13 +575,13 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.06381648560948316</v>
+        <v>0.04370309305202161</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>0.09906522325984961</v>
+        <v>0.1677989630732037</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>0.1603676101957249</v>
+        <v>0.07612722892127428</v>
       </c>
     </row>
     <row r="10">
@@ -591,13 +591,13 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.03389756153197578</v>
+        <v>0.1618585534500533</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>0.00909894069660629</v>
+        <v>0.09055126348683162</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>0.1472256226679706</v>
+        <v>0.04144314431805703</v>
       </c>
     </row>
     <row r="11">
@@ -607,13 +607,13 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.1003331034877064</v>
+        <v>0.049325297685688</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0.1425822847319283</v>
+        <v>0.0522258868704585</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>0.06986451533502785</v>
+        <v>0.1307142713125733</v>
       </c>
     </row>
     <row r="12">
@@ -623,13 +623,13 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.1649822475151234</v>
+        <v>0.1728481827133619</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>0.1211946650815522</v>
+        <v>0.02688413024126295</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>0.1022219488247707</v>
+        <v>0.107497903670104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update module to adjust new fleet
</commit_message>
<xml_diff>
--- a/Taxes_Factors.xlsx
+++ b/Taxes_Factors.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,11 +450,6 @@
           <t>FACTORS_2</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>FACTORS_3</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -463,13 +458,10 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.1273426742845834</v>
+        <v>0.07420953862125235</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>0.1375864719616154</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>0.009218662286240091</v>
+        <v>0.05024566007685418</v>
       </c>
     </row>
     <row r="3">
@@ -479,13 +471,10 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.1385664810060629</v>
+        <v>0.02681802474505173</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.07361601420459957</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>0.1608122037454987</v>
+        <v>0.0805501369649695</v>
       </c>
     </row>
     <row r="4">
@@ -495,13 +484,10 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>0.02866171107854141</v>
+        <v>0.01095802025131672</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.1286148203061389</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>0.1410991310337403</v>
+        <v>0.01392820978207283</v>
       </c>
     </row>
     <row r="5">
@@ -511,13 +497,10 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>0.005599852723031887</v>
+        <v>0.09491908165544634</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.0439363938074464</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>0.1681830836057347</v>
+        <v>0.1052733130998613</v>
       </c>
     </row>
     <row r="6">
@@ -527,13 +510,10 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.08988188957996833</v>
+        <v>0.1728148818351061</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0.1059079198305923</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>0.02792260181143307</v>
+        <v>0.04317076313937656</v>
       </c>
     </row>
     <row r="7">
@@ -543,13 +523,10 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.1108322445897598</v>
+        <v>0.140133896904935</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.1721514704028065</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>0.04982390814496991</v>
+        <v>0.1388960739136928</v>
       </c>
     </row>
     <row r="8">
@@ -559,13 +536,10 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.07138001983692742</v>
+        <v>0.1037968923310682</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0.0007266658150443441</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>0.08715786115037481</v>
+        <v>0.02661676147595037</v>
       </c>
     </row>
     <row r="9">
@@ -575,13 +549,10 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.04370309305202161</v>
+        <v>0.1259133810640778</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>0.1677989630732037</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>0.07612722892127428</v>
+        <v>0.1739457295677783</v>
       </c>
     </row>
     <row r="10">
@@ -591,13 +562,10 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.1618585534500533</v>
+        <v>0.1509661593483238</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>0.09055126348683162</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>0.04144314431805703</v>
+        <v>0.08775544229858545</v>
       </c>
     </row>
     <row r="11">
@@ -607,13 +575,10 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.049325297685688</v>
+        <v>0.0463592010248985</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0.0522258868704585</v>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>0.1307142713125733</v>
+        <v>0.1537747724949112</v>
       </c>
     </row>
     <row r="12">
@@ -623,13 +588,10 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.1728481827133619</v>
+        <v>0.05311092221852348</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>0.02688413024126295</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>0.107497903670104</v>
+        <v>0.1258431371859476</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add scrappage rate, experimental model
</commit_message>
<xml_diff>
--- a/Taxes_Factors.xlsx
+++ b/Taxes_Factors.xlsx
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.07420953862125235</v>
+        <v>0.1422929754124884</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>0.05024566007685418</v>
+        <v>0.06206059048872284</v>
       </c>
     </row>
     <row r="3">
@@ -471,10 +471,10 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.02681802474505173</v>
+        <v>0.07597668412866533</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.0805501369649695</v>
+        <v>0.1487447694034979</v>
       </c>
     </row>
     <row r="4">
@@ -484,10 +484,10 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>0.01095802025131672</v>
+        <v>0.01824749113468727</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.01392820978207283</v>
+        <v>0.07785249618475309</v>
       </c>
     </row>
     <row r="5">
@@ -497,10 +497,10 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>0.09491908165544634</v>
+        <v>0.1770615309149006</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.1052733130998613</v>
+        <v>0.007590897519115494</v>
       </c>
     </row>
     <row r="6">
@@ -510,10 +510,10 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.1728148818351061</v>
+        <v>0.1100476951253636</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0.04317076313937656</v>
+        <v>0.03442464693173394</v>
       </c>
     </row>
     <row r="7">
@@ -523,10 +523,10 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.140133896904935</v>
+        <v>0.09189774332174123</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.1388960739136928</v>
+        <v>0.1292786773499676</v>
       </c>
     </row>
     <row r="8">
@@ -536,10 +536,10 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.1037968923310682</v>
+        <v>0.04545117007920132</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0.02661676147595037</v>
+        <v>0.08896421609904119</v>
       </c>
     </row>
     <row r="9">
@@ -549,10 +549,10 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.1259133810640778</v>
+        <v>0.1271459160149058</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>0.1739457295677783</v>
+        <v>0.1454769433553602</v>
       </c>
     </row>
     <row r="10">
@@ -562,10 +562,10 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.1509661593483238</v>
+        <v>0.1511606971817293</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>0.08775544229858545</v>
+        <v>0.02595141623140635</v>
       </c>
     </row>
     <row r="11">
@@ -575,10 +575,10 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.0463592010248985</v>
+        <v>0.004122276361780318</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0.1537747724949112</v>
+        <v>0.110508344624508</v>
       </c>
     </row>
     <row r="12">
@@ -588,10 +588,10 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.05311092221852348</v>
+        <v>0.05659582032453687</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>0.1258431371859476</v>
+        <v>0.1691470018118935</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update version with last fleet and residual fleet changes
</commit_message>
<xml_diff>
--- a/Taxes_Factors.xlsx
+++ b/Taxes_Factors.xlsx
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.1422929754124884</v>
+        <v>0.05655663498788772</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>0.06206059048872284</v>
+        <v>0.1359908389070116</v>
       </c>
     </row>
     <row r="3">
@@ -471,10 +471,10 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.07597668412866533</v>
+        <v>0.02196328644039709</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.1487447694034979</v>
+        <v>0.1304520425990578</v>
       </c>
     </row>
     <row r="4">
@@ -484,10 +484,10 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>0.01824749113468727</v>
+        <v>0.04096965791260385</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.07785249618475309</v>
+        <v>0.008087151552221504</v>
       </c>
     </row>
     <row r="5">
@@ -497,10 +497,10 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>0.1770615309149006</v>
+        <v>0.0925062977245604</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.007590897519115494</v>
+        <v>0.1579197655247583</v>
       </c>
     </row>
     <row r="6">
@@ -510,10 +510,10 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.1100476951253636</v>
+        <v>0.1758902683728675</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0.03442464693173394</v>
+        <v>0.03647514590128042</v>
       </c>
     </row>
     <row r="7">
@@ -523,10 +523,10 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.09189774332174123</v>
+        <v>0.1377214964859611</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.1292786773499676</v>
+        <v>0.1010167672858878</v>
       </c>
     </row>
     <row r="8">
@@ -536,10 +536,10 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.04545117007920132</v>
+        <v>0.07295172638819263</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0.08896421609904119</v>
+        <v>0.0878713633355193</v>
       </c>
     </row>
     <row r="9">
@@ -549,10 +549,10 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.1271459160149058</v>
+        <v>0.1552345544195202</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>0.1454769433553602</v>
+        <v>0.03103785626392362</v>
       </c>
     </row>
     <row r="10">
@@ -562,10 +562,10 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.1511606971817293</v>
+        <v>0.1268263865293169</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>0.02595141623140635</v>
+        <v>0.08407575761679273</v>
       </c>
     </row>
     <row r="11">
@@ -575,10 +575,10 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.004122276361780318</v>
+        <v>0.00364600266289573</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0.110508344624508</v>
+        <v>0.169806166325199</v>
       </c>
     </row>
     <row r="12">
@@ -588,10 +588,10 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.05659582032453687</v>
+        <v>0.1157336880757968</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>0.1691470018118935</v>
+        <v>0.05726714468834777</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update with final experiment model
</commit_message>
<xml_diff>
--- a/Taxes_Factors.xlsx
+++ b/Taxes_Factors.xlsx
@@ -598,94 +598,94 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.1540883451658472</v>
+        <v>0.03871063961148565</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>0.0756770943281042</v>
+        <v>0.07477977070507996</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0.0142042758993839</v>
+        <v>0.06687892875342408</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0.02878143736760699</v>
+        <v>0.06924480420373909</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>0.07781925592819815</v>
+        <v>0.09735399216477204</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>0.1741991833315877</v>
+        <v>0.1417906130079702</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>0.0241068621551509</v>
+        <v>0.1338142373189911</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>0.1340529508580767</v>
+        <v>0.06066942668672094</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>0.08857305753991528</v>
+        <v>0.02994860923208943</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>0.1006899064073335</v>
+        <v>0.1357022032873653</v>
       </c>
       <c r="L2" s="2" t="n">
-        <v>0.07016926405031199</v>
+        <v>0.1473155972932792</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>0.08281980714961186</v>
+        <v>0.06200661076493105</v>
       </c>
       <c r="N2" s="2" t="n">
-        <v>0.1413540905967053</v>
+        <v>0.1073768867863662</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>0.05348522943370754</v>
+        <v>0.1215512946292413</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>0.1470977699945487</v>
+        <v>0.05475531488344264</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>0.1689188590328498</v>
+        <v>0.01783683861553111</v>
       </c>
       <c r="R2" s="2" t="n">
-        <v>0.173417364918811</v>
+        <v>0.1395175989953234</v>
       </c>
       <c r="S2" s="2" t="n">
-        <v>0.1757171119214633</v>
+        <v>0.164970544475512</v>
       </c>
       <c r="T2" s="2" t="n">
-        <v>0.07886475372661089</v>
+        <v>0.1542851093146232</v>
       </c>
       <c r="U2" s="2" t="n">
-        <v>0.0903617778216808</v>
+        <v>0.09492656023659204</v>
       </c>
       <c r="V2" s="2" t="n">
-        <v>0.1525338040379266</v>
+        <v>0.02754689498426848</v>
       </c>
       <c r="W2" s="2" t="n">
-        <v>0.1583180197068432</v>
+        <v>0.1337937771017354</v>
       </c>
       <c r="X2" s="2" t="n">
-        <v>0.1055011367478174</v>
+        <v>0.1083116040055895</v>
       </c>
       <c r="Y2" s="2" t="n">
-        <v>0.1042424095785772</v>
+        <v>0.03684695466013027</v>
       </c>
       <c r="Z2" s="2" t="n">
-        <v>0.106970261873519</v>
+        <v>0.1682104330693749</v>
       </c>
       <c r="AA2" s="2" t="n">
-        <v>0.1313545540481443</v>
+        <v>0.009868306037651936</v>
       </c>
       <c r="AB2" s="2" t="n">
-        <v>0.1240416882056928</v>
+        <v>0.1512764489746592</v>
       </c>
       <c r="AC2" s="2" t="n">
-        <v>0.1831476756754958</v>
+        <v>0.07622507206382821</v>
       </c>
       <c r="AD2" s="2" t="n">
-        <v>0.1796042163205821</v>
+        <v>0.02054861021220484</v>
       </c>
       <c r="AE2" s="2" t="n">
-        <v>0.05532880994595819</v>
+        <v>0.008767016009642558</v>
       </c>
     </row>
     <row r="3">
@@ -695,94 +695,94 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.08931944830740127</v>
+        <v>0.005314844333267501</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.01194092152020222</v>
+        <v>0.09287747774797883</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0.1093806420612908</v>
+        <v>0.1692542496504644</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.1319388670992276</v>
+        <v>0.0280707023140013</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0.146036858834474</v>
+        <v>0.1679534815884232</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>0.1522960003138611</v>
+        <v>0.08993037077030502</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>0.1612073013626337</v>
+        <v>0.05085114526024767</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>0.0759314565892413</v>
+        <v>0.1469745462410405</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>0.1048043674556566</v>
+        <v>0.07038530203689029</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>0.1525646818780977</v>
+        <v>0.1250284431531031</v>
       </c>
       <c r="L3" s="2" t="n">
-        <v>0.08659824815109857</v>
+        <v>0.04035654483484765</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>0.03360626479164892</v>
+        <v>0.06889864760306598</v>
       </c>
       <c r="N3" s="2" t="n">
-        <v>0.1709891820431835</v>
+        <v>0.0890801072999093</v>
       </c>
       <c r="O3" s="2" t="n">
-        <v>0.1585449129796196</v>
+        <v>0.01329918222789562</v>
       </c>
       <c r="P3" s="2" t="n">
-        <v>0.02428010859293137</v>
+        <v>0.08008754484692666</v>
       </c>
       <c r="Q3" s="2" t="n">
-        <v>0.08381747010405199</v>
+        <v>0.08402884922328875</v>
       </c>
       <c r="R3" s="2" t="n">
-        <v>0.01451906413814441</v>
+        <v>0.1214020264834413</v>
       </c>
       <c r="S3" s="2" t="n">
-        <v>0.0003459116462098396</v>
+        <v>0.1430113567415627</v>
       </c>
       <c r="T3" s="2" t="n">
-        <v>0.1003765232317791</v>
+        <v>0.1125254790620522</v>
       </c>
       <c r="U3" s="2" t="n">
-        <v>0.1385768333993247</v>
+        <v>0.08125237850253889</v>
       </c>
       <c r="V3" s="2" t="n">
-        <v>0.1503261015698466</v>
+        <v>0.1430145650864267</v>
       </c>
       <c r="W3" s="2" t="n">
-        <v>0.03177034372261321</v>
+        <v>0.1408903485289979</v>
       </c>
       <c r="X3" s="2" t="n">
-        <v>0.07399511596326962</v>
+        <v>0.0126683037557617</v>
       </c>
       <c r="Y3" s="2" t="n">
-        <v>0.1465868129685775</v>
+        <v>0.1516025149120511</v>
       </c>
       <c r="Z3" s="2" t="n">
-        <v>0.03393751920616662</v>
+        <v>0.1574330348123151</v>
       </c>
       <c r="AA3" s="2" t="n">
-        <v>0.1570486053517914</v>
+        <v>0.04340458156079872</v>
       </c>
       <c r="AB3" s="2" t="n">
-        <v>0.08515535060012674</v>
+        <v>0.09169482147845714</v>
       </c>
       <c r="AC3" s="2" t="n">
-        <v>0.1273379918714126</v>
+        <v>0.110350654289125</v>
       </c>
       <c r="AD3" s="2" t="n">
-        <v>0.1429493078544422</v>
+        <v>0.01431797428811986</v>
       </c>
       <c r="AE3" s="2" t="n">
-        <v>0.09243364538868404</v>
+        <v>0.0281083190712976</v>
       </c>
     </row>
     <row r="4">
@@ -792,94 +792,94 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>0.03821150464882874</v>
+        <v>0.08625595417511212</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.06464435905035379</v>
+        <v>0.01989723999000774</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0.1197898974589161</v>
+        <v>0.06580390619438804</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>0.03618109000609759</v>
+        <v>0.1515616172901827</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>0.1197306841787757</v>
+        <v>0.1006504269087745</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>0.1360959136775817</v>
+        <v>0.05866071925500729</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>0.01605089591649212</v>
+        <v>0.0885806945491756</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>0.09107861783224128</v>
+        <v>0.1157472134067222</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>0.1463075002714963</v>
+        <v>0.006552555805147396</v>
       </c>
       <c r="K4" s="2" t="n">
-        <v>0.001912919525940558</v>
+        <v>0.1524968335292128</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>0.1701848150919439</v>
+        <v>0.1751493098531763</v>
       </c>
       <c r="M4" s="2" t="n">
-        <v>0.0226306944760718</v>
+        <v>0.1841701042018216</v>
       </c>
       <c r="N4" s="2" t="n">
-        <v>0.07087327899572578</v>
+        <v>0.1465185844798714</v>
       </c>
       <c r="O4" s="2" t="n">
-        <v>0.1771695752123678</v>
+        <v>0.1405354501175066</v>
       </c>
       <c r="P4" s="2" t="n">
-        <v>0.06961713057620141</v>
+        <v>0.003297872274305178</v>
       </c>
       <c r="Q4" s="2" t="n">
-        <v>0.1579652898357963</v>
+        <v>0.1470913771384185</v>
       </c>
       <c r="R4" s="2" t="n">
-        <v>0.08359211589525647</v>
+        <v>0.09376528607495489</v>
       </c>
       <c r="S4" s="2" t="n">
-        <v>0.08032414154132038</v>
+        <v>0.01140945134008042</v>
       </c>
       <c r="T4" s="2" t="n">
-        <v>0.1499333329296441</v>
+        <v>0.1399345719529894</v>
       </c>
       <c r="U4" s="2" t="n">
-        <v>0.1578252181219117</v>
+        <v>0.1171851593283262</v>
       </c>
       <c r="V4" s="2" t="n">
-        <v>0.03602000416518664</v>
+        <v>0.08563022020084451</v>
       </c>
       <c r="W4" s="2" t="n">
-        <v>0.08933682771200464</v>
+        <v>0.02544472403450405</v>
       </c>
       <c r="X4" s="2" t="n">
-        <v>0.1700042091860235</v>
+        <v>0.05184940595380824</v>
       </c>
       <c r="Y4" s="2" t="n">
-        <v>0.06726260569620522</v>
+        <v>0.06041612624100642</v>
       </c>
       <c r="Z4" s="2" t="n">
-        <v>0.1777185358904818</v>
+        <v>0.02170124595711635</v>
       </c>
       <c r="AA4" s="2" t="n">
-        <v>0.06664169434693891</v>
+        <v>0.09267987883240554</v>
       </c>
       <c r="AB4" s="2" t="n">
-        <v>0.1483519007229176</v>
+        <v>0.1056297539759618</v>
       </c>
       <c r="AC4" s="2" t="n">
-        <v>0.01424648332290337</v>
+        <v>0.1366202722270315</v>
       </c>
       <c r="AD4" s="2" t="n">
-        <v>0.06033120674622624</v>
+        <v>0.04657943857352522</v>
       </c>
       <c r="AE4" s="2" t="n">
-        <v>0.04384315015475339</v>
+        <v>0.06085561608089615</v>
       </c>
     </row>
     <row r="5">
@@ -889,94 +889,94 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>0.1773023468104303</v>
+        <v>0.1404200595919835</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.0842650512539548</v>
+        <v>0.1574628460967909</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>0.05969464821646954</v>
+        <v>0.04090596727475775</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>0.06422762596847197</v>
+        <v>0.09882111561977848</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>0.004450025648144138</v>
+        <v>0.02785009229080204</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>0.08505086325248101</v>
+        <v>0.04772282960204545</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>0.1359098061568723</v>
+        <v>0.04528662089756617</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>0.1089143747431625</v>
+        <v>0.008690533956011487</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>0.123405297724425</v>
+        <v>0.1322927713694043</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>0.08323331962654795</v>
+        <v>0.1666605297027562</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>0.1047159788953305</v>
+        <v>0.1178650571204542</v>
       </c>
       <c r="M5" s="2" t="n">
-        <v>0.08149913252090019</v>
+        <v>0.1360357303276798</v>
       </c>
       <c r="N5" s="2" t="n">
-        <v>0.009712855824215567</v>
+        <v>0.001633690225528421</v>
       </c>
       <c r="O5" s="2" t="n">
-        <v>0.001568183490602402</v>
+        <v>0.03881179501267</v>
       </c>
       <c r="P5" s="2" t="n">
-        <v>0.08573253456379905</v>
+        <v>0.1715618140730495</v>
       </c>
       <c r="Q5" s="2" t="n">
-        <v>0.02025912360134293</v>
+        <v>0.00728741967888815</v>
       </c>
       <c r="R5" s="2" t="n">
-        <v>0.02061209690878541</v>
+        <v>0.1760504745955005</v>
       </c>
       <c r="S5" s="2" t="n">
-        <v>0.08758014591968133</v>
+        <v>0.05395106072030561</v>
       </c>
       <c r="T5" s="2" t="n">
-        <v>0.1427946611954189</v>
+        <v>0.002813864414977231</v>
       </c>
       <c r="U5" s="2" t="n">
-        <v>0.1080544861046762</v>
+        <v>0.02299481228724192</v>
       </c>
       <c r="V5" s="2" t="n">
-        <v>0.1170244795314667</v>
+        <v>0.0332506427995586</v>
       </c>
       <c r="W5" s="2" t="n">
-        <v>0.002462844674530429</v>
+        <v>0.07039145389027544</v>
       </c>
       <c r="X5" s="2" t="n">
-        <v>0.02164872554444235</v>
+        <v>0.07194109736967619</v>
       </c>
       <c r="Y5" s="2" t="n">
-        <v>0.04087637157844898</v>
+        <v>0.1100633517404452</v>
       </c>
       <c r="Z5" s="2" t="n">
-        <v>0.1591329993480325</v>
+        <v>0.07920476231919535</v>
       </c>
       <c r="AA5" s="2" t="n">
-        <v>0.1094364196008413</v>
+        <v>0.1173193840555757</v>
       </c>
       <c r="AB5" s="2" t="n">
-        <v>0.1561194019400632</v>
+        <v>0.1457294642629566</v>
       </c>
       <c r="AC5" s="2" t="n">
-        <v>0.08372850366140662</v>
+        <v>0.06449757676156027</v>
       </c>
       <c r="AD5" s="2" t="n">
-        <v>0.02306937725277488</v>
+        <v>0.05782041805379001</v>
       </c>
       <c r="AE5" s="2" t="n">
-        <v>0.1399248489261492</v>
+        <v>0.1730321280932862</v>
       </c>
     </row>
     <row r="6">
@@ -986,94 +986,94 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.10282621601866</v>
+        <v>0.06795907336061585</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0.136851498629758</v>
+        <v>0.1184700688225971</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0.1702202122763242</v>
+        <v>0.02862730533458849</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>0.172822870576664</v>
+        <v>0.09303130201456099</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0.09824811478483776</v>
+        <v>0.001785292091841568</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>0.06069885243586921</v>
+        <v>0.1033676473705805</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>0.1198054741162213</v>
+        <v>0.1835805432272684</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>0.03780351300533822</v>
+        <v>0.1202481527677263</v>
       </c>
       <c r="J6" s="2" t="n">
-        <v>0.05447905201357922</v>
+        <v>0.05946948356154313</v>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0.134871380722677</v>
+        <v>0.07523150176965511</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>0.04431998898046833</v>
+        <v>0.02944823234751314</v>
       </c>
       <c r="M6" s="2" t="n">
-        <v>0.009277216949131114</v>
+        <v>0.04536785426160345</v>
       </c>
       <c r="N6" s="2" t="n">
-        <v>0.1307589148984845</v>
+        <v>0.1231426051181173</v>
       </c>
       <c r="O6" s="2" t="n">
-        <v>0.1149531195420762</v>
+        <v>0.05837136335430779</v>
       </c>
       <c r="P6" s="2" t="n">
-        <v>0.105057265401389</v>
+        <v>0.1405928225636587</v>
       </c>
       <c r="Q6" s="2" t="n">
-        <v>0.1501623111448207</v>
+        <v>0.175048830383097</v>
       </c>
       <c r="R6" s="2" t="n">
-        <v>0.05834138280707169</v>
+        <v>0.1098509584805479</v>
       </c>
       <c r="S6" s="2" t="n">
-        <v>0.04256924626877702</v>
+        <v>0.09146903780629061</v>
       </c>
       <c r="T6" s="2" t="n">
-        <v>0.1317208398648874</v>
+        <v>0.01971012369820041</v>
       </c>
       <c r="U6" s="2" t="n">
-        <v>0.124717792272809</v>
+        <v>0.04163868656350696</v>
       </c>
       <c r="V6" s="2" t="n">
-        <v>0.0635979745170492</v>
+        <v>0.1752279634491429</v>
       </c>
       <c r="W6" s="2" t="n">
-        <v>0.0611745893866245</v>
+        <v>0.1550465887174072</v>
       </c>
       <c r="X6" s="2" t="n">
-        <v>0.08770014042278319</v>
+        <v>0.0849402403278323</v>
       </c>
       <c r="Y6" s="2" t="n">
-        <v>0.1236037205426787</v>
+        <v>0.03149286155628221</v>
       </c>
       <c r="Z6" s="2" t="n">
-        <v>0.005675739227729876</v>
+        <v>0.1162646140411216</v>
       </c>
       <c r="AA6" s="2" t="n">
-        <v>0.0264914931809208</v>
+        <v>0.02914314419005381</v>
       </c>
       <c r="AB6" s="2" t="n">
-        <v>0.08131661436428489</v>
+        <v>0.05516673439228106</v>
       </c>
       <c r="AC6" s="2" t="n">
-        <v>0.05476887901315667</v>
+        <v>0.02333405116386256</v>
       </c>
       <c r="AD6" s="2" t="n">
-        <v>0.1535930314059261</v>
+        <v>0.1080047746181484</v>
       </c>
       <c r="AE6" s="2" t="n">
-        <v>0.09901562355358863</v>
+        <v>0.04235095792181114</v>
       </c>
     </row>
     <row r="7">
@@ -1083,94 +1083,94 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.01068676607042268</v>
+        <v>0.03069689249220979</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.1774875246046848</v>
+        <v>0.1724311911575778</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0.152846685590422</v>
+        <v>0.1050119777483555</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>0.10348182368082</v>
+        <v>0.1741366865032962</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>0.05594516869562595</v>
+        <v>0.06171461670822695</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>0.03942587518635748</v>
+        <v>0.07453737136888051</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>0.1122094339117148</v>
+        <v>0.164351924643619</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>0.123488898714907</v>
+        <v>0.02338919812721185</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>0.04018641815886408</v>
+        <v>0.1715945316987712</v>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.04437647960170612</v>
+        <v>0.1096192001979419</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>0.05412594908108845</v>
+        <v>0.09157763116567189</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>0.1778267714513154</v>
+        <v>0.1323272354126204</v>
       </c>
       <c r="N7" s="2" t="n">
-        <v>0.05656122899733055</v>
+        <v>0.0472601804652294</v>
       </c>
       <c r="O7" s="2" t="n">
-        <v>0.1379286983224301</v>
+        <v>0.1728959327293133</v>
       </c>
       <c r="P7" s="2" t="n">
-        <v>0.06031097511873531</v>
+        <v>0.04232388011057911</v>
       </c>
       <c r="Q7" s="2" t="n">
-        <v>0.08100119964360128</v>
+        <v>0.1025782380204451</v>
       </c>
       <c r="R7" s="2" t="n">
-        <v>0.1455513645216993</v>
+        <v>0.003377205354851335</v>
       </c>
       <c r="S7" s="2" t="n">
-        <v>0.05348097780779947</v>
+        <v>0.1053851438699311</v>
       </c>
       <c r="T7" s="2" t="n">
-        <v>0.1786997986588797</v>
+        <v>0.1771496988394921</v>
       </c>
       <c r="U7" s="2" t="n">
-        <v>0.07091765785780686</v>
+        <v>0.165799251035587</v>
       </c>
       <c r="V7" s="2" t="n">
-        <v>0.1166029728792716</v>
+        <v>0.1583100175793626</v>
       </c>
       <c r="W7" s="2" t="n">
-        <v>0.1011710793910956</v>
+        <v>0.1705084158511384</v>
       </c>
       <c r="X7" s="2" t="n">
-        <v>0.1476164209063966</v>
+        <v>0.1568362819965006</v>
       </c>
       <c r="Y7" s="2" t="n">
-        <v>0.1785900381753829</v>
+        <v>0.1379615656746097</v>
       </c>
       <c r="Z7" s="2" t="n">
-        <v>0.01952405237254878</v>
+        <v>0.008400540712449285</v>
       </c>
       <c r="AA7" s="2" t="n">
-        <v>0.04781085960751204</v>
+        <v>0.153394268337254</v>
       </c>
       <c r="AB7" s="2" t="n">
-        <v>0.1709720651573477</v>
+        <v>0.1757456727074025</v>
       </c>
       <c r="AC7" s="2" t="n">
-        <v>0.1344768835627818</v>
+        <v>0.1258380949476148</v>
       </c>
       <c r="AD7" s="2" t="n">
-        <v>0.1206666725617367</v>
+        <v>0.0968760079548588</v>
       </c>
       <c r="AE7" s="2" t="n">
-        <v>0.1606847761966093</v>
+        <v>0.08328052986870507</v>
       </c>
     </row>
     <row r="8">
@@ -1180,94 +1180,94 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.1403119718055936</v>
+        <v>0.09904989420187001</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0.02278432979788437</v>
+        <v>0.03474792649365909</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>0.07367035969954953</v>
+        <v>0.1229813547902525</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>0.0962863590828055</v>
+        <v>0.01364404796732597</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>0.1671494032620021</v>
+        <v>0.1591245902518887</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>0.06752399860594442</v>
+        <v>0.1190540446897561</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>0.08435438030871442</v>
+        <v>0.1171334940151913</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>0.1770351018520703</v>
+        <v>0.03360258800275655</v>
       </c>
       <c r="J8" s="2" t="n">
-        <v>0.07050458089934535</v>
+        <v>0.08913005218096887</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.1308205651817842</v>
+        <v>0.08687558511193924</v>
       </c>
       <c r="L8" s="2" t="n">
-        <v>0.006786718157698573</v>
+        <v>0.0113990858022005</v>
       </c>
       <c r="M8" s="2" t="n">
-        <v>0.1257055890929648</v>
+        <v>0.1552675245480059</v>
       </c>
       <c r="N8" s="2" t="n">
-        <v>0.02712573991884087</v>
+        <v>0.1587008395942116</v>
       </c>
       <c r="O8" s="2" t="n">
-        <v>0.04749717873794279</v>
+        <v>0.03097637243306694</v>
       </c>
       <c r="P8" s="2" t="n">
-        <v>0.03482926830488375</v>
+        <v>0.1338062546611663</v>
       </c>
       <c r="Q8" s="2" t="n">
-        <v>0.1227195253061167</v>
+        <v>0.05197816431296045</v>
       </c>
       <c r="R8" s="2" t="n">
-        <v>0.04513205078221905</v>
+        <v>0.07212553054976702</v>
       </c>
       <c r="S8" s="2" t="n">
-        <v>0.1423387836993741</v>
+        <v>0.1215704853244753</v>
       </c>
       <c r="T8" s="2" t="n">
-        <v>0.05173684752228995</v>
+        <v>0.1237287276224732</v>
       </c>
       <c r="U8" s="2" t="n">
-        <v>0.04308200906907442</v>
+        <v>0.1565749103751878</v>
       </c>
       <c r="V8" s="2" t="n">
-        <v>0.01679467737448634</v>
+        <v>0.05614164539901433</v>
       </c>
       <c r="W8" s="2" t="n">
-        <v>0.03585616360503602</v>
+        <v>0.05696663301230811</v>
       </c>
       <c r="X8" s="2" t="n">
-        <v>0.06015800984395442</v>
+        <v>0.02731497157558319</v>
       </c>
       <c r="Y8" s="2" t="n">
-        <v>0.05234853709662161</v>
+        <v>0.09290002310720635</v>
       </c>
       <c r="Z8" s="2" t="n">
-        <v>0.059946701318584</v>
+        <v>0.1463843092286806</v>
       </c>
       <c r="AA8" s="2" t="n">
-        <v>0.08824173187178319</v>
+        <v>0.1347466681235822</v>
       </c>
       <c r="AB8" s="2" t="n">
-        <v>0.1058610960200598</v>
+        <v>0.0005699710522821105</v>
       </c>
       <c r="AC8" s="2" t="n">
-        <v>0.1074991327715147</v>
+        <v>0.1666674940697451</v>
       </c>
       <c r="AD8" s="2" t="n">
-        <v>0.0001293088366122582</v>
+        <v>0.0759824738919453</v>
       </c>
       <c r="AE8" s="2" t="n">
-        <v>0.1731955353525281</v>
+        <v>0.118446252550025</v>
       </c>
     </row>
     <row r="9">
@@ -1277,94 +1277,94 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.05447165207886328</v>
+        <v>0.1601352882554084</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>0.16184611399097</v>
+        <v>0.005657206295752092</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>0.03637781430211176</v>
+        <v>0.1628618413485931</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>0.0729492466984135</v>
+        <v>0.05931280282966504</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>0.1543495654053324</v>
+        <v>0.1300074676205573</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>0.01627126144515779</v>
+        <v>0.0228695428651623</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>0.07525434375116599</v>
+        <v>0.003823550215903765</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>0.002715278573130455</v>
+        <v>0.1547187013802047</v>
       </c>
       <c r="J9" s="2" t="n">
-        <v>0.02927783551081891</v>
+        <v>0.03625180819855039</v>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.1761772546507556</v>
+        <v>0.05742995920558841</v>
       </c>
       <c r="L9" s="2" t="n">
-        <v>0.1255190449581572</v>
+        <v>0.05555074590041875</v>
       </c>
       <c r="M9" s="2" t="n">
-        <v>0.05631061790617339</v>
+        <v>0.08700004861332236</v>
       </c>
       <c r="N9" s="2" t="n">
-        <v>0.1099458258431895</v>
+        <v>0.1734740443298893</v>
       </c>
       <c r="O9" s="2" t="n">
-        <v>0.1172834066877912</v>
+        <v>0.1534598954571779</v>
       </c>
       <c r="P9" s="2" t="n">
-        <v>0.0104608304496994</v>
+        <v>0.1038283517602142</v>
       </c>
       <c r="Q9" s="2" t="n">
-        <v>0.1119069209722226</v>
+        <v>0.1272154649820232</v>
       </c>
       <c r="R9" s="2" t="n">
-        <v>0.0768349775094139</v>
+        <v>0.02988599430097761</v>
       </c>
       <c r="S9" s="2" t="n">
-        <v>0.1257935689842196</v>
+        <v>0.06978768651818591</v>
       </c>
       <c r="T9" s="2" t="n">
-        <v>0.04068810453650544</v>
+        <v>0.09612049759984166</v>
       </c>
       <c r="U9" s="2" t="n">
-        <v>0.06603311360162827</v>
+        <v>0.1367307133544809</v>
       </c>
       <c r="V9" s="2" t="n">
-        <v>0.005829290027163512</v>
+        <v>0.07123390721710643</v>
       </c>
       <c r="W9" s="2" t="n">
-        <v>0.1800224689304381</v>
+        <v>0.1165424333526189</v>
       </c>
       <c r="X9" s="2" t="n">
-        <v>0.125929754957407</v>
+        <v>0.1399524061214249</v>
       </c>
       <c r="Y9" s="2" t="n">
-        <v>0.008030637480513459</v>
+        <v>0.008922305715060053</v>
       </c>
       <c r="Z9" s="2" t="n">
-        <v>0.09271397415861843</v>
+        <v>0.06492997892754533</v>
       </c>
       <c r="AA9" s="2" t="n">
-        <v>0.1246056329203453</v>
+        <v>0.06302890092671362</v>
       </c>
       <c r="AB9" s="2" t="n">
-        <v>0.05369667266548097</v>
+        <v>0.01951446574937863</v>
       </c>
       <c r="AC9" s="2" t="n">
-        <v>0.04585325796973891</v>
+        <v>0.1530315589814703</v>
       </c>
       <c r="AD9" s="2" t="n">
-        <v>0.1123183537899262</v>
+        <v>0.1342098599226059</v>
       </c>
       <c r="AE9" s="2" t="n">
-        <v>0.006569828242097485</v>
+        <v>0.1150641984734777</v>
       </c>
     </row>
     <row r="10">
@@ -1374,94 +1374,94 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.03007455921805473</v>
+        <v>0.176509085037836</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>0.03870868174212567</v>
+        <v>0.1214626924643529</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>0.09310218793521535</v>
+        <v>0.01016620103718973</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>0.1634415391673066</v>
+        <v>0.1411553991091462</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0.02387175386076182</v>
+        <v>0.1348108425935858</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>0.02943172922825225</v>
+        <v>0.159971891315808</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>0.1664551228851501</v>
+        <v>0.08295716733721784</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>0.1614954042211884</v>
+        <v>0.09873871651864254</v>
       </c>
       <c r="J10" s="2" t="n">
-        <v>0.01545542756460362</v>
+        <v>0.1402669103758812</v>
       </c>
       <c r="K10" s="2" t="n">
-        <v>0.1000361333844847</v>
+        <v>0.03188067784454556</v>
       </c>
       <c r="L10" s="2" t="n">
-        <v>0.1598291975489975</v>
+        <v>0.07537902589930955</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>0.1537048366240724</v>
+        <v>0.104536288288425</v>
       </c>
       <c r="N10" s="2" t="n">
-        <v>0.1535367404788486</v>
+        <v>0.02493549028772704</v>
       </c>
       <c r="O10" s="2" t="n">
-        <v>0.02027435216727048</v>
+        <v>0.07613813538390882</v>
       </c>
       <c r="P10" s="2" t="n">
-        <v>0.1797672701180278</v>
+        <v>0.1558173984416878</v>
       </c>
       <c r="Q10" s="2" t="n">
-        <v>0.05565874546747727</v>
+        <v>0.08056814985549508</v>
       </c>
       <c r="R10" s="2" t="n">
-        <v>0.1486901425047191</v>
+        <v>0.04225170995071378</v>
       </c>
       <c r="S10" s="2" t="n">
-        <v>0.161730473356337</v>
+        <v>0.03385632100531082</v>
       </c>
       <c r="T10" s="2" t="n">
-        <v>0.02443277183565744</v>
+        <v>0.06449799284097704</v>
       </c>
       <c r="U10" s="2" t="n">
-        <v>0.1686003129732901</v>
+        <v>0.1076635492552392</v>
       </c>
       <c r="V10" s="2" t="n">
-        <v>0.09774525283626817</v>
+        <v>0.1277596677028441</v>
       </c>
       <c r="W10" s="2" t="n">
-        <v>0.148307318240859</v>
+        <v>0.006222523370325661</v>
       </c>
       <c r="X10" s="2" t="n">
-        <v>0.01082542044941675</v>
+        <v>0.1243595621567934</v>
       </c>
       <c r="Y10" s="2" t="n">
-        <v>0.09892041385972584</v>
+        <v>0.1748189922092386</v>
       </c>
       <c r="Z10" s="2" t="n">
-        <v>0.1343161273982144</v>
+        <v>0.03911623476260839</v>
       </c>
       <c r="AA10" s="2" t="n">
-        <v>0.1720991576828828</v>
+        <v>0.07341145606329574</v>
       </c>
       <c r="AB10" s="2" t="n">
-        <v>0.03738045497172248</v>
+        <v>0.07754591624909096</v>
       </c>
       <c r="AC10" s="2" t="n">
-        <v>0.01818693672366398</v>
+        <v>0.008008958677150185</v>
       </c>
       <c r="AD10" s="2" t="n">
-        <v>0.03942332723800813</v>
+        <v>0.1237037285517557</v>
       </c>
       <c r="AE10" s="2" t="n">
-        <v>0.08014523592805389</v>
+        <v>0.1425152723435145</v>
       </c>
     </row>
     <row r="11">
@@ -1471,94 +1471,94 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.1237471408997562</v>
+        <v>0.1300049829238696</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0.1003350427361777</v>
+        <v>0.05958173028860094</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>0.1418663789115803</v>
+        <v>0.1413279266009781</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.001624333864075326</v>
+        <v>0.0449082851977312</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>0.04163181091276734</v>
+        <v>0.04272756334375311</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>0.1290603732603602</v>
+        <v>0.01511967368315216</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>0.06203698309426703</v>
+        <v>0.02860451708615378</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>0.05562363311520403</v>
+        <v>0.06658160471598004</v>
       </c>
       <c r="J11" s="2" t="n">
-        <v>0.1751833881607812</v>
+        <v>0.158772973192715</v>
       </c>
       <c r="K11" s="2" t="n">
-        <v>0.05361439574674171</v>
+        <v>0.04322549455852826</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>0.03187476700852528</v>
+        <v>0.1124674684894525</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>0.1099848833136138</v>
+        <v>0.001339837227811974</v>
       </c>
       <c r="N11" s="2" t="n">
-        <v>0.03686406639206705</v>
+        <v>0.07311262234434951</v>
       </c>
       <c r="O11" s="2" t="n">
-        <v>0.07785072266996518</v>
+        <v>0.0894765650074239</v>
       </c>
       <c r="P11" s="2" t="n">
-        <v>0.161388284730252</v>
+        <v>0.09411914984602268</v>
       </c>
       <c r="Q11" s="2" t="n">
-        <v>0.01345611365198255</v>
+        <v>0.04826743490164432</v>
       </c>
       <c r="R11" s="2" t="n">
-        <v>0.1104251967996474</v>
+        <v>0.1510298527109761</v>
       </c>
       <c r="S11" s="2" t="n">
-        <v>0.02331024745477178</v>
+        <v>0.02477961995193363</v>
       </c>
       <c r="T11" s="2" t="n">
-        <v>0.09478263546339573</v>
+        <v>0.03809499554178065</v>
       </c>
       <c r="U11" s="2" t="n">
-        <v>0.02086882426425758</v>
+        <v>0.01090453610469194</v>
       </c>
       <c r="V11" s="2" t="n">
-        <v>0.1715701235972745</v>
+        <v>0.01223268267548048</v>
       </c>
       <c r="W11" s="2" t="n">
-        <v>0.07552510397434757</v>
+        <v>0.03673126418974719</v>
       </c>
       <c r="X11" s="2" t="n">
-        <v>0.0430621981144352</v>
+        <v>0.177452216023806</v>
       </c>
       <c r="Y11" s="2" t="n">
-        <v>0.01794542137811126</v>
+        <v>0.1263278581485054</v>
       </c>
       <c r="Z11" s="2" t="n">
-        <v>0.1311747007463516</v>
+        <v>0.1036097401929034</v>
       </c>
       <c r="AA11" s="2" t="n">
-        <v>0.01565905305820946</v>
+        <v>0.1063874952982999</v>
       </c>
       <c r="AB11" s="2" t="n">
-        <v>0.0157247177767041</v>
+        <v>0.04732095398476309</v>
       </c>
       <c r="AC11" s="2" t="n">
-        <v>0.1561725447864458</v>
+        <v>0.0963971135303504</v>
       </c>
       <c r="AD11" s="2" t="n">
-        <v>0.07912883135276969</v>
+        <v>0.1481985825734533</v>
       </c>
       <c r="AE11" s="2" t="n">
-        <v>0.1229753871686722</v>
+        <v>0.06685509732879218</v>
       </c>
     </row>
     <row r="12">
@@ -1568,94 +1568,94 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.07896004897614212</v>
+        <v>0.06494328601634158</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>0.1254593823457844</v>
+        <v>0.1426318499376028</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>0.02884689764873671</v>
+        <v>0.08618034126700837</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0.128264806488511</v>
+        <v>0.1261132369505726</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>0.1107673584890808</v>
+        <v>0.076021634437375</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>0.109945949262547</v>
+        <v>0.1669752960713323</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>0.04260939634161729</v>
+        <v>0.1010161054486656</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>0.03186077049543991</v>
+        <v>0.1706393181969828</v>
       </c>
       <c r="J12" s="2" t="n">
-        <v>0.1518230747005145</v>
+        <v>0.1053350023480388</v>
       </c>
       <c r="K12" s="2" t="n">
-        <v>0.02170296327393091</v>
+        <v>0.01584957163936409</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>0.1458760280763796</v>
+        <v>0.1434913012936764</v>
       </c>
       <c r="M12" s="2" t="n">
-        <v>0.1466341857244962</v>
+        <v>0.02305011875071239</v>
       </c>
       <c r="N12" s="2" t="n">
-        <v>0.09227807601140869</v>
+        <v>0.05476494906880067</v>
       </c>
       <c r="O12" s="2" t="n">
-        <v>0.09344462075622659</v>
+        <v>0.1044840136474882</v>
       </c>
       <c r="P12" s="2" t="n">
-        <v>0.1214585621495322</v>
+        <v>0.01980959653894733</v>
       </c>
       <c r="Q12" s="2" t="n">
-        <v>0.03413444123973762</v>
+        <v>0.1580992328882084</v>
       </c>
       <c r="R12" s="2" t="n">
-        <v>0.1228842432142323</v>
+        <v>0.06074336250294613</v>
       </c>
       <c r="S12" s="2" t="n">
-        <v>0.1068093914000462</v>
+        <v>0.1798092922464118</v>
       </c>
       <c r="T12" s="2" t="n">
-        <v>0.005969731034931265</v>
+        <v>0.07113893911259302</v>
       </c>
       <c r="U12" s="2" t="n">
-        <v>0.01096197451354045</v>
+        <v>0.06432944295660702</v>
       </c>
       <c r="V12" s="2" t="n">
-        <v>0.07195531946406007</v>
+        <v>0.1096517929059509</v>
       </c>
       <c r="W12" s="2" t="n">
-        <v>0.1160552406556076</v>
+        <v>0.08746183795094162</v>
       </c>
       <c r="X12" s="2" t="n">
-        <v>0.153558867864054</v>
+        <v>0.0443739107132241</v>
       </c>
       <c r="Y12" s="2" t="n">
-        <v>0.1615930316451573</v>
+        <v>0.06864744603546484</v>
       </c>
       <c r="Z12" s="2" t="n">
-        <v>0.07888938845975303</v>
+        <v>0.09474510597668963</v>
       </c>
       <c r="AA12" s="2" t="n">
-        <v>0.06061079833063038</v>
+        <v>0.1766159165743689</v>
       </c>
       <c r="AB12" s="2" t="n">
-        <v>0.02138003757559962</v>
+        <v>0.1298057971727669</v>
       </c>
       <c r="AC12" s="2" t="n">
-        <v>0.07458171064147985</v>
+        <v>0.03902915328826164</v>
       </c>
       <c r="AD12" s="2" t="n">
-        <v>0.08878636664099562</v>
+        <v>0.1737581313595926</v>
       </c>
       <c r="AE12" s="2" t="n">
-        <v>0.02588315914290579</v>
+        <v>0.160724612258552</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clean and update general module
</commit_message>
<xml_diff>
--- a/Taxes_Factors.xlsx
+++ b/Taxes_Factors.xlsx
@@ -598,94 +598,94 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.03871063961148565</v>
+        <v>0.07171576342679235</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>0.07477977070507996</v>
+        <v>0.1231095124134499</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0.06687892875342408</v>
+        <v>0.01442235779825341</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0.06924480420373909</v>
+        <v>0.06781223861961475</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>0.09735399216477204</v>
+        <v>0.04258959361787915</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>0.1417906130079702</v>
+        <v>0.04916333320278912</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>0.1338142373189911</v>
+        <v>0.09910220002944969</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>0.06066942668672094</v>
+        <v>0.1433358990667638</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>0.02994860923208943</v>
+        <v>0.1408486234491142</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>0.1357022032873653</v>
+        <v>0.07703533952511381</v>
       </c>
       <c r="L2" s="2" t="n">
-        <v>0.1473155972932792</v>
+        <v>0.05745689002198571</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>0.06200661076493105</v>
+        <v>0.09143187646243438</v>
       </c>
       <c r="N2" s="2" t="n">
-        <v>0.1073768867863662</v>
+        <v>0.03161105655606015</v>
       </c>
       <c r="O2" s="2" t="n">
-        <v>0.1215512946292413</v>
+        <v>0.07792974704272325</v>
       </c>
       <c r="P2" s="2" t="n">
-        <v>0.05475531488344264</v>
+        <v>0.02849457669500938</v>
       </c>
       <c r="Q2" s="2" t="n">
-        <v>0.01783683861553111</v>
+        <v>0.04435770053408628</v>
       </c>
       <c r="R2" s="2" t="n">
-        <v>0.1395175989953234</v>
+        <v>0.09496551510188342</v>
       </c>
       <c r="S2" s="2" t="n">
-        <v>0.164970544475512</v>
+        <v>0.1378342022728268</v>
       </c>
       <c r="T2" s="2" t="n">
-        <v>0.1542851093146232</v>
+        <v>0.08711012729533431</v>
       </c>
       <c r="U2" s="2" t="n">
-        <v>0.09492656023659204</v>
+        <v>0.1690728002970778</v>
       </c>
       <c r="V2" s="2" t="n">
-        <v>0.02754689498426848</v>
+        <v>0.1066133728012709</v>
       </c>
       <c r="W2" s="2" t="n">
-        <v>0.1337937771017354</v>
+        <v>0.07614937706911071</v>
       </c>
       <c r="X2" s="2" t="n">
-        <v>0.1083116040055895</v>
+        <v>0.1418825775972027</v>
       </c>
       <c r="Y2" s="2" t="n">
-        <v>0.03684695466013027</v>
+        <v>0.1503576924894071</v>
       </c>
       <c r="Z2" s="2" t="n">
-        <v>0.1682104330693749</v>
+        <v>0.02624742739128959</v>
       </c>
       <c r="AA2" s="2" t="n">
-        <v>0.009868306037651936</v>
+        <v>0.139993785584471</v>
       </c>
       <c r="AB2" s="2" t="n">
-        <v>0.1512764489746592</v>
+        <v>0.04835774994519708</v>
       </c>
       <c r="AC2" s="2" t="n">
-        <v>0.07622507206382821</v>
+        <v>0.1125160991908456</v>
       </c>
       <c r="AD2" s="2" t="n">
-        <v>0.02054861021220484</v>
+        <v>0.1643516690579858</v>
       </c>
       <c r="AE2" s="2" t="n">
-        <v>0.008767016009642558</v>
+        <v>0.03328426090800188</v>
       </c>
     </row>
     <row r="3">
@@ -695,94 +695,94 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.005314844333267501</v>
+        <v>0.09705414115317196</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.09287747774797883</v>
+        <v>0.02908680198160287</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0.1692542496504644</v>
+        <v>0.06989799429130614</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.0280707023140013</v>
+        <v>0.1119032269419595</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0.1679534815884232</v>
+        <v>0.1651684586282407</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>0.08993037077030502</v>
+        <v>0.1692244963915083</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>0.05085114526024767</v>
+        <v>0.05491076173182843</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>0.1469745462410405</v>
+        <v>0.002170935615547073</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>0.07038530203689029</v>
+        <v>0.1639571970282902</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>0.1250284431531031</v>
+        <v>0.006654131710174792</v>
       </c>
       <c r="L3" s="2" t="n">
-        <v>0.04035654483484765</v>
+        <v>0.06679472772877296</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>0.06889864760306598</v>
+        <v>0.105386788141498</v>
       </c>
       <c r="N3" s="2" t="n">
-        <v>0.0890801072999093</v>
+        <v>0.03989246752150657</v>
       </c>
       <c r="O3" s="2" t="n">
-        <v>0.01329918222789562</v>
+        <v>0.09169493992248856</v>
       </c>
       <c r="P3" s="2" t="n">
-        <v>0.08008754484692666</v>
+        <v>0.1435562734203138</v>
       </c>
       <c r="Q3" s="2" t="n">
-        <v>0.08402884922328875</v>
+        <v>0.07990749180904341</v>
       </c>
       <c r="R3" s="2" t="n">
-        <v>0.1214020264834413</v>
+        <v>0.1157383170741011</v>
       </c>
       <c r="S3" s="2" t="n">
-        <v>0.1430113567415627</v>
+        <v>0.05675569662599309</v>
       </c>
       <c r="T3" s="2" t="n">
-        <v>0.1125254790620522</v>
+        <v>0.1174877713661177</v>
       </c>
       <c r="U3" s="2" t="n">
-        <v>0.08125237850253889</v>
+        <v>0.1310046569800448</v>
       </c>
       <c r="V3" s="2" t="n">
-        <v>0.1430145650864267</v>
+        <v>0.1521552623119827</v>
       </c>
       <c r="W3" s="2" t="n">
-        <v>0.1408903485289979</v>
+        <v>0.1580192010284661</v>
       </c>
       <c r="X3" s="2" t="n">
-        <v>0.0126683037557617</v>
+        <v>0.09461222761358121</v>
       </c>
       <c r="Y3" s="2" t="n">
-        <v>0.1516025149120511</v>
+        <v>0.1051223949800099</v>
       </c>
       <c r="Z3" s="2" t="n">
-        <v>0.1574330348123151</v>
+        <v>0.06467525987592927</v>
       </c>
       <c r="AA3" s="2" t="n">
-        <v>0.04340458156079872</v>
+        <v>0.1139688434899584</v>
       </c>
       <c r="AB3" s="2" t="n">
-        <v>0.09169482147845714</v>
+        <v>0.1007048898387181</v>
       </c>
       <c r="AC3" s="2" t="n">
-        <v>0.110350654289125</v>
+        <v>0.01584685611714173</v>
       </c>
       <c r="AD3" s="2" t="n">
-        <v>0.01431797428811986</v>
+        <v>0.1009498657409151</v>
       </c>
       <c r="AE3" s="2" t="n">
-        <v>0.0281083190712976</v>
+        <v>0.007263448571913478</v>
       </c>
     </row>
     <row r="4">
@@ -792,94 +792,94 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>0.08625595417511212</v>
+        <v>0.1651368758904573</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.01989723999000774</v>
+        <v>0.006865053808413476</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0.06580390619438804</v>
+        <v>0.1026970717496638</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>0.1515616172901827</v>
+        <v>0.1386442595252734</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>0.1006504269087745</v>
+        <v>0.02135622016635454</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>0.05866071925500729</v>
+        <v>0.1505626864377196</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>0.0885806945491756</v>
+        <v>0.1394275351688449</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>0.1157472134067222</v>
+        <v>0.1227070187253644</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>0.006552555805147396</v>
+        <v>0.101511282082079</v>
       </c>
       <c r="K4" s="2" t="n">
-        <v>0.1524968335292128</v>
+        <v>0.05939491215953675</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>0.1751493098531763</v>
+        <v>0.1150544819107006</v>
       </c>
       <c r="M4" s="2" t="n">
-        <v>0.1841701042018216</v>
+        <v>0.02378051971727498</v>
       </c>
       <c r="N4" s="2" t="n">
-        <v>0.1465185844798714</v>
+        <v>0.01451490465792421</v>
       </c>
       <c r="O4" s="2" t="n">
-        <v>0.1405354501175066</v>
+        <v>0.06146457462433085</v>
       </c>
       <c r="P4" s="2" t="n">
-        <v>0.003297872274305178</v>
+        <v>0.09399745862827841</v>
       </c>
       <c r="Q4" s="2" t="n">
-        <v>0.1470913771384185</v>
+        <v>0.1697874560754973</v>
       </c>
       <c r="R4" s="2" t="n">
-        <v>0.09376528607495489</v>
+        <v>0.05495576983701592</v>
       </c>
       <c r="S4" s="2" t="n">
-        <v>0.01140945134008042</v>
+        <v>0.08052769855093875</v>
       </c>
       <c r="T4" s="2" t="n">
-        <v>0.1399345719529894</v>
+        <v>0.01172685055342821</v>
       </c>
       <c r="U4" s="2" t="n">
-        <v>0.1171851593283262</v>
+        <v>0.05937468480348267</v>
       </c>
       <c r="V4" s="2" t="n">
-        <v>0.08563022020084451</v>
+        <v>0.01278695585568113</v>
       </c>
       <c r="W4" s="2" t="n">
-        <v>0.02544472403450405</v>
+        <v>0.02734583421176418</v>
       </c>
       <c r="X4" s="2" t="n">
-        <v>0.05184940595380824</v>
+        <v>0.04917193494295558</v>
       </c>
       <c r="Y4" s="2" t="n">
-        <v>0.06041612624100642</v>
+        <v>0.08396555899983227</v>
       </c>
       <c r="Z4" s="2" t="n">
-        <v>0.02170124595711635</v>
+        <v>0.09508877461029798</v>
       </c>
       <c r="AA4" s="2" t="n">
-        <v>0.09267987883240554</v>
+        <v>0.1713578074926129</v>
       </c>
       <c r="AB4" s="2" t="n">
-        <v>0.1056297539759618</v>
+        <v>0.00722183362831896</v>
       </c>
       <c r="AC4" s="2" t="n">
-        <v>0.1366202722270315</v>
+        <v>0.116501612310369</v>
       </c>
       <c r="AD4" s="2" t="n">
-        <v>0.04657943857352522</v>
+        <v>0.08741505602692351</v>
       </c>
       <c r="AE4" s="2" t="n">
-        <v>0.06085561608089615</v>
+        <v>0.03129348126582072</v>
       </c>
     </row>
     <row r="5">
@@ -889,94 +889,94 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>0.1404200595919835</v>
+        <v>0.03538792749277432</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.1574628460967909</v>
+        <v>0.1412329777173588</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>0.04090596727475775</v>
+        <v>0.05232974339532836</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>0.09882111561977848</v>
+        <v>0.0369899320793266</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>0.02785009229080204</v>
+        <v>0.08802519401460666</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>0.04772282960204545</v>
+        <v>0.07445637834768534</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>0.04528662089756617</v>
+        <v>0.1584627737660426</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>0.008690533956011487</v>
+        <v>0.1560828817309969</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>0.1322927713694043</v>
+        <v>0.09821056486358684</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>0.1666605297027562</v>
+        <v>0.02508154794478681</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>0.1178650571204542</v>
+        <v>0.001997957559860472</v>
       </c>
       <c r="M5" s="2" t="n">
-        <v>0.1360357303276798</v>
+        <v>0.1382237714422946</v>
       </c>
       <c r="N5" s="2" t="n">
-        <v>0.001633690225528421</v>
+        <v>0.05035298838577285</v>
       </c>
       <c r="O5" s="2" t="n">
-        <v>0.03881179501267</v>
+        <v>0.1234743168923644</v>
       </c>
       <c r="P5" s="2" t="n">
-        <v>0.1715618140730495</v>
+        <v>0.01385878938250273</v>
       </c>
       <c r="Q5" s="2" t="n">
-        <v>0.00728741967888815</v>
+        <v>0.1155137538139261</v>
       </c>
       <c r="R5" s="2" t="n">
-        <v>0.1760504745955005</v>
+        <v>0.0758284441510092</v>
       </c>
       <c r="S5" s="2" t="n">
-        <v>0.05395106072030561</v>
+        <v>0.01925374371286717</v>
       </c>
       <c r="T5" s="2" t="n">
-        <v>0.002813864414977231</v>
+        <v>0.1828514986014157</v>
       </c>
       <c r="U5" s="2" t="n">
-        <v>0.02299481228724192</v>
+        <v>0.03121490925161854</v>
       </c>
       <c r="V5" s="2" t="n">
-        <v>0.0332506427995586</v>
+        <v>0.06087414016243547</v>
       </c>
       <c r="W5" s="2" t="n">
-        <v>0.07039145389027544</v>
+        <v>0.09426552436857394</v>
       </c>
       <c r="X5" s="2" t="n">
-        <v>0.07194109736967619</v>
+        <v>0.1678076987600131</v>
       </c>
       <c r="Y5" s="2" t="n">
-        <v>0.1100633517404452</v>
+        <v>0.05876886078560555</v>
       </c>
       <c r="Z5" s="2" t="n">
-        <v>0.07920476231919535</v>
+        <v>0.1284954317076894</v>
       </c>
       <c r="AA5" s="2" t="n">
-        <v>0.1173193840555757</v>
+        <v>0.09678317532227686</v>
       </c>
       <c r="AB5" s="2" t="n">
-        <v>0.1457294642629566</v>
+        <v>0.06244520983307028</v>
       </c>
       <c r="AC5" s="2" t="n">
-        <v>0.06449757676156027</v>
+        <v>0.0524314869262206</v>
       </c>
       <c r="AD5" s="2" t="n">
-        <v>0.05782041805379001</v>
+        <v>0.0686633629528883</v>
       </c>
       <c r="AE5" s="2" t="n">
-        <v>0.1730321280932862</v>
+        <v>0.06945822345725487</v>
       </c>
     </row>
     <row r="6">
@@ -986,94 +986,94 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.06795907336061585</v>
+        <v>0.1672090612105084</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0.1184700688225971</v>
+        <v>0.1116367914655521</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0.02862730533458849</v>
+        <v>0.03782042485919446</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>0.09303130201456099</v>
+        <v>0.1612581462766603</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0.001785292091841568</v>
+        <v>0.06836826879208795</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>0.1033676473705805</v>
+        <v>0.1185246224943724</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>0.1835805432272684</v>
+        <v>0.02988591999685881</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>0.1202481527677263</v>
+        <v>0.04785425107881796</v>
       </c>
       <c r="J6" s="2" t="n">
-        <v>0.05946948356154313</v>
+        <v>0.1283754002305549</v>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0.07523150176965511</v>
+        <v>0.04094270458480383</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>0.02944823234751314</v>
+        <v>0.0295658487487446</v>
       </c>
       <c r="M6" s="2" t="n">
-        <v>0.04536785426160345</v>
+        <v>0.1713573774586379</v>
       </c>
       <c r="N6" s="2" t="n">
-        <v>0.1231426051181173</v>
+        <v>0.07157295956809666</v>
       </c>
       <c r="O6" s="2" t="n">
-        <v>0.05837136335430779</v>
+        <v>0.1506307984628091</v>
       </c>
       <c r="P6" s="2" t="n">
-        <v>0.1405928225636587</v>
+        <v>0.1596052319118039</v>
       </c>
       <c r="Q6" s="2" t="n">
-        <v>0.175048830383097</v>
+        <v>0.05984157529488741</v>
       </c>
       <c r="R6" s="2" t="n">
-        <v>0.1098509584805479</v>
+        <v>0.01602019494555187</v>
       </c>
       <c r="S6" s="2" t="n">
-        <v>0.09146903780629061</v>
+        <v>0.1234535035251386</v>
       </c>
       <c r="T6" s="2" t="n">
-        <v>0.01971012369820041</v>
+        <v>0.1076766500075697</v>
       </c>
       <c r="U6" s="2" t="n">
-        <v>0.04163868656350696</v>
+        <v>0.03381860405993435</v>
       </c>
       <c r="V6" s="2" t="n">
-        <v>0.1752279634491429</v>
+        <v>0.09239956795842724</v>
       </c>
       <c r="W6" s="2" t="n">
-        <v>0.1550465887174072</v>
+        <v>0.04313006308813866</v>
       </c>
       <c r="X6" s="2" t="n">
-        <v>0.0849402403278323</v>
+        <v>0.06109632598090912</v>
       </c>
       <c r="Y6" s="2" t="n">
-        <v>0.03149286155628221</v>
+        <v>0.1742775855546788</v>
       </c>
       <c r="Z6" s="2" t="n">
-        <v>0.1162646140411216</v>
+        <v>0.1612529363552425</v>
       </c>
       <c r="AA6" s="2" t="n">
-        <v>0.02914314419005381</v>
+        <v>0.1233522712884713</v>
       </c>
       <c r="AB6" s="2" t="n">
-        <v>0.05516673439228106</v>
+        <v>0.130994650125997</v>
       </c>
       <c r="AC6" s="2" t="n">
-        <v>0.02333405116386256</v>
+        <v>0.06737511707775638</v>
       </c>
       <c r="AD6" s="2" t="n">
-        <v>0.1080047746181484</v>
+        <v>0.1434219674518036</v>
       </c>
       <c r="AE6" s="2" t="n">
-        <v>0.04235095792181114</v>
+        <v>0.1144333319338501</v>
       </c>
     </row>
     <row r="7">
@@ -1083,94 +1083,94 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.03069689249220979</v>
+        <v>0.0497323034073614</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.1724311911575778</v>
+        <v>0.09240623730726456</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0.1050119777483555</v>
+        <v>0.1669801778952365</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>0.1741366865032962</v>
+        <v>0.1716351640185551</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>0.06171461670822695</v>
+        <v>0.1646008370425912</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>0.07453737136888051</v>
+        <v>0.02348921830280849</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>0.164351924643619</v>
+        <v>0.166461650153709</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>0.02338919812721185</v>
+        <v>0.06132386270726901</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>0.1715945316987712</v>
+        <v>0.05386206260557069</v>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.1096192001979419</v>
+        <v>0.1219776236137813</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>0.09157763116567189</v>
+        <v>0.1459607946627237</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>0.1323272354126204</v>
+        <v>0.1253141345749871</v>
       </c>
       <c r="N7" s="2" t="n">
-        <v>0.0472601804652294</v>
+        <v>0.1154993423722225</v>
       </c>
       <c r="O7" s="2" t="n">
-        <v>0.1728959327293133</v>
+        <v>0.1064199722985767</v>
       </c>
       <c r="P7" s="2" t="n">
-        <v>0.04232388011057911</v>
+        <v>0.1686341583544731</v>
       </c>
       <c r="Q7" s="2" t="n">
-        <v>0.1025782380204451</v>
+        <v>0.009014605278927829</v>
       </c>
       <c r="R7" s="2" t="n">
-        <v>0.003377205354851335</v>
+        <v>0.1682278982031404</v>
       </c>
       <c r="S7" s="2" t="n">
-        <v>0.1053851438699311</v>
+        <v>0.03584254443003855</v>
       </c>
       <c r="T7" s="2" t="n">
-        <v>0.1771496988394921</v>
+        <v>0.07100274962125822</v>
       </c>
       <c r="U7" s="2" t="n">
-        <v>0.165799251035587</v>
+        <v>0.09249725195880984</v>
       </c>
       <c r="V7" s="2" t="n">
-        <v>0.1583100175793626</v>
+        <v>0.1407132897256062</v>
       </c>
       <c r="W7" s="2" t="n">
-        <v>0.1705084158511384</v>
+        <v>0.01041556937330695</v>
       </c>
       <c r="X7" s="2" t="n">
-        <v>0.1568362819965006</v>
+        <v>0.07584371893723454</v>
       </c>
       <c r="Y7" s="2" t="n">
-        <v>0.1379615656746097</v>
+        <v>0.07570164727946277</v>
       </c>
       <c r="Z7" s="2" t="n">
-        <v>0.008400540712449285</v>
+        <v>0.1346749723055508</v>
       </c>
       <c r="AA7" s="2" t="n">
-        <v>0.153394268337254</v>
+        <v>0.05776460118801569</v>
       </c>
       <c r="AB7" s="2" t="n">
-        <v>0.1757456727074025</v>
+        <v>0.180487968601701</v>
       </c>
       <c r="AC7" s="2" t="n">
-        <v>0.1258380949476148</v>
+        <v>0.1650562769048773</v>
       </c>
       <c r="AD7" s="2" t="n">
-        <v>0.0968760079548588</v>
+        <v>0.1174416789344632</v>
       </c>
       <c r="AE7" s="2" t="n">
-        <v>0.08328052986870507</v>
+        <v>0.1473509192647244</v>
       </c>
     </row>
     <row r="8">
@@ -1180,94 +1180,94 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.09904989420187001</v>
+        <v>0.02944216264734621</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0.03474792649365909</v>
+        <v>0.1539578694221797</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>0.1229813547902525</v>
+        <v>0.1215947994413354</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>0.01364404796732597</v>
+        <v>0.09738456430701775</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>0.1591245902518887</v>
+        <v>0.1270787123453894</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>0.1190540446897561</v>
+        <v>0.09869492190083592</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>0.1171334940151913</v>
+        <v>0.01129189000068609</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>0.03360258800275655</v>
+        <v>0.09921463017880233</v>
       </c>
       <c r="J8" s="2" t="n">
-        <v>0.08913005218096887</v>
+        <v>0.0372557288079246</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.08687558511193924</v>
+        <v>0.1608688795411638</v>
       </c>
       <c r="L8" s="2" t="n">
-        <v>0.0113990858022005</v>
+        <v>0.129472247696173</v>
       </c>
       <c r="M8" s="2" t="n">
-        <v>0.1552675245480059</v>
+        <v>0.08250857086167977</v>
       </c>
       <c r="N8" s="2" t="n">
-        <v>0.1587008395942116</v>
+        <v>0.1067830599568574</v>
       </c>
       <c r="O8" s="2" t="n">
-        <v>0.03097637243306694</v>
+        <v>0.1712023187796675</v>
       </c>
       <c r="P8" s="2" t="n">
-        <v>0.1338062546611663</v>
+        <v>0.04488156783722042</v>
       </c>
       <c r="Q8" s="2" t="n">
-        <v>0.05197816431296045</v>
+        <v>0.02208304696715004</v>
       </c>
       <c r="R8" s="2" t="n">
-        <v>0.07212553054976702</v>
+        <v>0.02504692494592457</v>
       </c>
       <c r="S8" s="2" t="n">
-        <v>0.1215704853244753</v>
+        <v>0.009116107596225147</v>
       </c>
       <c r="T8" s="2" t="n">
-        <v>0.1237287276224732</v>
+        <v>0.1448274769502954</v>
       </c>
       <c r="U8" s="2" t="n">
-        <v>0.1565749103751878</v>
+        <v>0.002774040831129634</v>
       </c>
       <c r="V8" s="2" t="n">
-        <v>0.05614164539901433</v>
+        <v>0.07435233205268967</v>
       </c>
       <c r="W8" s="2" t="n">
-        <v>0.05696663301230811</v>
+        <v>0.1684827205880873</v>
       </c>
       <c r="X8" s="2" t="n">
-        <v>0.02731497157558319</v>
+        <v>0.01149998821630767</v>
       </c>
       <c r="Y8" s="2" t="n">
-        <v>0.09290002310720635</v>
+        <v>0.04883349604479238</v>
       </c>
       <c r="Z8" s="2" t="n">
-        <v>0.1463843092286806</v>
+        <v>0.0724328226258576</v>
       </c>
       <c r="AA8" s="2" t="n">
-        <v>0.1347466681235822</v>
+        <v>0.03774414839235606</v>
       </c>
       <c r="AB8" s="2" t="n">
-        <v>0.0005699710522821105</v>
+        <v>0.1358945477190084</v>
       </c>
       <c r="AC8" s="2" t="n">
-        <v>0.1666674940697451</v>
+        <v>0.03206781272792796</v>
       </c>
       <c r="AD8" s="2" t="n">
-        <v>0.0759824738919453</v>
+        <v>0.04634907395952851</v>
       </c>
       <c r="AE8" s="2" t="n">
-        <v>0.118446252550025</v>
+        <v>0.09414308031521668</v>
       </c>
     </row>
     <row r="9">
@@ -1277,94 +1277,94 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.1601352882554084</v>
+        <v>0.128524794076715</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>0.005657206295752092</v>
+        <v>0.0750703121911583</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>0.1628618413485931</v>
+        <v>0.1704940366803529</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>0.05931280282966504</v>
+        <v>0.02001877677410405</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>0.1300074676205573</v>
+        <v>0.1078760350240238</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>0.0228695428651623</v>
+        <v>0.06077338211330321</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>0.003823550215903765</v>
+        <v>0.1167034030136473</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>0.1547187013802047</v>
+        <v>0.02064046397234315</v>
       </c>
       <c r="J9" s="2" t="n">
-        <v>0.03625180819855039</v>
+        <v>0.182755111682449</v>
       </c>
       <c r="K9" s="2" t="n">
-        <v>0.05742995920558841</v>
+        <v>0.1373242864836041</v>
       </c>
       <c r="L9" s="2" t="n">
-        <v>0.05555074590041875</v>
+        <v>0.1567858671311467</v>
       </c>
       <c r="M9" s="2" t="n">
-        <v>0.08700004861332236</v>
+        <v>0.03583996733603029</v>
       </c>
       <c r="N9" s="2" t="n">
-        <v>0.1734740443298893</v>
+        <v>0.09374248323410701</v>
       </c>
       <c r="O9" s="2" t="n">
-        <v>0.1534598954571779</v>
+        <v>0.01577821909928195</v>
       </c>
       <c r="P9" s="2" t="n">
-        <v>0.1038283517602142</v>
+        <v>0.1240722238728227</v>
       </c>
       <c r="Q9" s="2" t="n">
-        <v>0.1272154649820232</v>
+        <v>0.1436194879760242</v>
       </c>
       <c r="R9" s="2" t="n">
-        <v>0.02988599430097761</v>
+        <v>0.1556789591661658</v>
       </c>
       <c r="S9" s="2" t="n">
-        <v>0.06978768651818591</v>
+        <v>0.1572942572874015</v>
       </c>
       <c r="T9" s="2" t="n">
-        <v>0.09612049759984166</v>
+        <v>0.05999537226087357</v>
       </c>
       <c r="U9" s="2" t="n">
-        <v>0.1367307133544809</v>
+        <v>0.1077671064463964</v>
       </c>
       <c r="V9" s="2" t="n">
-        <v>0.07123390721710643</v>
+        <v>0.1731038202314113</v>
       </c>
       <c r="W9" s="2" t="n">
-        <v>0.1165424333526189</v>
+        <v>0.05133227714627597</v>
       </c>
       <c r="X9" s="2" t="n">
-        <v>0.1399524061214249</v>
+        <v>0.1546475365752971</v>
       </c>
       <c r="Y9" s="2" t="n">
-        <v>0.008922305715060053</v>
+        <v>0.1586025818645276</v>
       </c>
       <c r="Z9" s="2" t="n">
-        <v>0.06492997892754533</v>
+        <v>0.1029338620468798</v>
       </c>
       <c r="AA9" s="2" t="n">
-        <v>0.06302890092671362</v>
+        <v>0.009225915931177407</v>
       </c>
       <c r="AB9" s="2" t="n">
-        <v>0.01951446574937863</v>
+        <v>0.06801070143507237</v>
       </c>
       <c r="AC9" s="2" t="n">
-        <v>0.1530315589814703</v>
+        <v>0.159985874163499</v>
       </c>
       <c r="AD9" s="2" t="n">
-        <v>0.1342098599226059</v>
+        <v>0.05976975480943018</v>
       </c>
       <c r="AE9" s="2" t="n">
-        <v>0.1150641984734777</v>
+        <v>0.1522440689393464</v>
       </c>
     </row>
     <row r="10">
@@ -1374,94 +1374,94 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.176509085037836</v>
+        <v>0.1423079333534337</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>0.1214626924643529</v>
+        <v>0.03427000056718667</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>0.01016620103718973</v>
+        <v>0.1460419572170461</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>0.1411553991091462</v>
+        <v>0.0029337571206955</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0.1348108425935858</v>
+        <v>0.05086111291833906</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>0.159971891315808</v>
+        <v>0.1041447034823968</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>0.08295716733721784</v>
+        <v>0.07893643991236601</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>0.09873871651864254</v>
+        <v>0.1004890052221642</v>
       </c>
       <c r="J10" s="2" t="n">
-        <v>0.1402669103758812</v>
+        <v>0.01784209162805594</v>
       </c>
       <c r="K10" s="2" t="n">
-        <v>0.03188067784454556</v>
+        <v>0.1653575035184282</v>
       </c>
       <c r="L10" s="2" t="n">
-        <v>0.07537902589930955</v>
+        <v>0.04224141520330988</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>0.104536288288425</v>
+        <v>0.1659649118010562</v>
       </c>
       <c r="N10" s="2" t="n">
-        <v>0.02493549028772704</v>
+        <v>0.145779368551408</v>
       </c>
       <c r="O10" s="2" t="n">
-        <v>0.07613813538390882</v>
+        <v>0.0218610278782904</v>
       </c>
       <c r="P10" s="2" t="n">
-        <v>0.1558173984416878</v>
+        <v>0.06861517630509066</v>
       </c>
       <c r="Q10" s="2" t="n">
-        <v>0.08056814985549508</v>
+        <v>0.1083657169177526</v>
       </c>
       <c r="R10" s="2" t="n">
-        <v>0.04225170995071378</v>
+        <v>0.1397754164661932</v>
       </c>
       <c r="S10" s="2" t="n">
-        <v>0.03385632100531082</v>
+        <v>0.0959790209982227</v>
       </c>
       <c r="T10" s="2" t="n">
-        <v>0.06449799284097704</v>
+        <v>0.1567913791639538</v>
       </c>
       <c r="U10" s="2" t="n">
-        <v>0.1076635492552392</v>
+        <v>0.1399118497243931</v>
       </c>
       <c r="V10" s="2" t="n">
-        <v>0.1277596677028441</v>
+        <v>0.1215630130078199</v>
       </c>
       <c r="W10" s="2" t="n">
-        <v>0.006222523370325661</v>
+        <v>0.1026051821530523</v>
       </c>
       <c r="X10" s="2" t="n">
-        <v>0.1243595621567934</v>
+        <v>0.01906769409094261</v>
       </c>
       <c r="Y10" s="2" t="n">
-        <v>0.1748189922092386</v>
+        <v>0.0231434824736523</v>
       </c>
       <c r="Z10" s="2" t="n">
-        <v>0.03911623476260839</v>
+        <v>0.009364801561553919</v>
       </c>
       <c r="AA10" s="2" t="n">
-        <v>0.07341145606329574</v>
+        <v>0.1500503225662802</v>
       </c>
       <c r="AB10" s="2" t="n">
-        <v>0.07754591624909096</v>
+        <v>0.0223640597532834</v>
       </c>
       <c r="AC10" s="2" t="n">
-        <v>0.008008958677150185</v>
+        <v>0.1416887599476599</v>
       </c>
       <c r="AD10" s="2" t="n">
-        <v>0.1237037285517557</v>
+        <v>0.0257248937302921</v>
       </c>
       <c r="AE10" s="2" t="n">
-        <v>0.1425152723435145</v>
+        <v>0.1653868853680832</v>
       </c>
     </row>
     <row r="11">
@@ -1471,94 +1471,94 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.1300049829238696</v>
+        <v>0.01142827517423278</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0.05958173028860094</v>
+        <v>0.1680705133093612</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>0.1413279266009781</v>
+        <v>0.03194613791624627</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.0449082851977312</v>
+        <v>0.06041822226931636</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>0.04272756334375311</v>
+        <v>0.1480506310988173</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>0.01511967368315216</v>
+        <v>0.003736509869991703</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>0.02860451708615378</v>
+        <v>0.1092939987845889</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>0.06658160471598004</v>
+        <v>0.07131085319682162</v>
       </c>
       <c r="J11" s="2" t="n">
-        <v>0.158772973192715</v>
+        <v>0.004473307169497693</v>
       </c>
       <c r="K11" s="2" t="n">
-        <v>0.04322549455852826</v>
+        <v>0.09691979288510585</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>0.1124674684894525</v>
+        <v>0.08337952532529973</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>0.001339837227811974</v>
+        <v>0.05408243532330655</v>
       </c>
       <c r="N11" s="2" t="n">
-        <v>0.07311262234434951</v>
+        <v>0.169236755744927</v>
       </c>
       <c r="O11" s="2" t="n">
-        <v>0.0894765650074239</v>
+        <v>0.04068153955526005</v>
       </c>
       <c r="P11" s="2" t="n">
-        <v>0.09411914984602268</v>
+        <v>0.05697889736933094</v>
       </c>
       <c r="Q11" s="2" t="n">
-        <v>0.04826743490164432</v>
+        <v>0.158896861656093</v>
       </c>
       <c r="R11" s="2" t="n">
-        <v>0.1510298527109761</v>
+        <v>0.1107418748148347</v>
       </c>
       <c r="S11" s="2" t="n">
-        <v>0.02477961995193363</v>
+        <v>0.1049352286102384</v>
       </c>
       <c r="T11" s="2" t="n">
-        <v>0.03809499554178065</v>
+        <v>0.03982720042459534</v>
       </c>
       <c r="U11" s="2" t="n">
-        <v>0.01090453610469194</v>
+        <v>0.1624110359339433</v>
       </c>
       <c r="V11" s="2" t="n">
-        <v>0.01223268267548048</v>
+        <v>0.02993985755469269</v>
       </c>
       <c r="W11" s="2" t="n">
-        <v>0.03673126418974719</v>
+        <v>0.1289780246182968</v>
       </c>
       <c r="X11" s="2" t="n">
-        <v>0.177452216023806</v>
+        <v>0.1247959583263838</v>
       </c>
       <c r="Y11" s="2" t="n">
-        <v>0.1263278581485054</v>
+        <v>0.0007405715459627622</v>
       </c>
       <c r="Z11" s="2" t="n">
-        <v>0.1036097401929034</v>
+        <v>0.03476978423991104</v>
       </c>
       <c r="AA11" s="2" t="n">
-        <v>0.1063874952982999</v>
+        <v>0.06841258948410774</v>
       </c>
       <c r="AB11" s="2" t="n">
-        <v>0.04732095398476309</v>
+        <v>0.1532172158381394</v>
       </c>
       <c r="AC11" s="2" t="n">
-        <v>0.0963971135303504</v>
+        <v>0.09306440388634031</v>
       </c>
       <c r="AD11" s="2" t="n">
-        <v>0.1481985825734533</v>
+        <v>0.00971169681696871</v>
       </c>
       <c r="AE11" s="2" t="n">
-        <v>0.06685509732879218</v>
+        <v>0.1290825346042636</v>
       </c>
     </row>
     <row r="12">
@@ -1568,94 +1568,94 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.06494328601634158</v>
+        <v>0.1020607621672066</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>0.1426318499376028</v>
+        <v>0.06429392981647238</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>0.08618034126700837</v>
+        <v>0.08577529875603673</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0.1261132369505726</v>
+        <v>0.1310017120674767</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>0.076021634437375</v>
+        <v>0.01602493635167051</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>0.1669752960713323</v>
+        <v>0.1472297474565891</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>0.1010161054486656</v>
+        <v>0.03552342744197828</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>0.1706393181969828</v>
+        <v>0.1748701985051094</v>
       </c>
       <c r="J12" s="2" t="n">
-        <v>0.1053350023480388</v>
+        <v>0.07090863045287703</v>
       </c>
       <c r="K12" s="2" t="n">
-        <v>0.01584957163936409</v>
+        <v>0.1084432780335008</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>0.1434913012936764</v>
+        <v>0.1712902440112828</v>
       </c>
       <c r="M12" s="2" t="n">
-        <v>0.02305011875071239</v>
+        <v>0.006109646880800151</v>
       </c>
       <c r="N12" s="2" t="n">
-        <v>0.05476494906880067</v>
+        <v>0.1610146134511176</v>
       </c>
       <c r="O12" s="2" t="n">
-        <v>0.1044840136474882</v>
+        <v>0.1388625454442071</v>
       </c>
       <c r="P12" s="2" t="n">
-        <v>0.01980959653894733</v>
+        <v>0.09730564622315413</v>
       </c>
       <c r="Q12" s="2" t="n">
-        <v>0.1580992328882084</v>
+        <v>0.08861230367661169</v>
       </c>
       <c r="R12" s="2" t="n">
-        <v>0.06074336250294613</v>
+        <v>0.04302068529417968</v>
       </c>
       <c r="S12" s="2" t="n">
-        <v>0.1798092922464118</v>
+        <v>0.1790079963901092</v>
       </c>
       <c r="T12" s="2" t="n">
-        <v>0.07113893911259302</v>
+        <v>0.02070292375515795</v>
       </c>
       <c r="U12" s="2" t="n">
-        <v>0.06432944295660702</v>
+        <v>0.0701530597131696</v>
       </c>
       <c r="V12" s="2" t="n">
-        <v>0.1096517929059509</v>
+        <v>0.03549838833798295</v>
       </c>
       <c r="W12" s="2" t="n">
-        <v>0.08746183795094162</v>
+        <v>0.139276226354927</v>
       </c>
       <c r="X12" s="2" t="n">
-        <v>0.0443739107132241</v>
+        <v>0.09957433895917267</v>
       </c>
       <c r="Y12" s="2" t="n">
-        <v>0.06864744603546484</v>
+        <v>0.1204861279820686</v>
       </c>
       <c r="Z12" s="2" t="n">
-        <v>0.09474510597668963</v>
+        <v>0.1700639272797981</v>
       </c>
       <c r="AA12" s="2" t="n">
-        <v>0.1766159165743689</v>
+        <v>0.03134653926027238</v>
       </c>
       <c r="AB12" s="2" t="n">
-        <v>0.1298057971727669</v>
+        <v>0.09030117328149388</v>
       </c>
       <c r="AC12" s="2" t="n">
-        <v>0.03902915328826164</v>
+        <v>0.04346570074736223</v>
       </c>
       <c r="AD12" s="2" t="n">
-        <v>0.1737581313595926</v>
+        <v>0.1762009805188011</v>
       </c>
       <c r="AE12" s="2" t="n">
-        <v>0.160724612258552</v>
+        <v>0.0560597653715247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>